<commit_message>
RTM: defects are fixed.
</commit_message>
<xml_diff>
--- a/src/com/accenture/tmt/Quality_Tracker/TMT_Defect_List & Summary.xlsx
+++ b/src/com/accenture/tmt/Quality_Tracker/TMT_Defect_List & Summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="18180" windowHeight="10245" tabRatio="575" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="13095" windowHeight="4665" tabRatio="575" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="17" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="346">
   <si>
     <t>Expected Result</t>
   </si>
@@ -2262,7 +2262,7 @@
   <sheetPr codeName="Sheet7">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A2:O52"/>
+  <dimension ref="B2:O52"/>
   <sheetViews>
     <sheetView topLeftCell="E18" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
@@ -3146,8 +3146,8 @@
   </sheetPr>
   <dimension ref="A1:EN122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="S98" sqref="S98"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="S96" sqref="S96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6657,7 +6657,9 @@
       <c r="R96" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="S96" s="55"/>
+      <c r="S96" s="71" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="97" spans="1:19" s="64" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="55">
@@ -6692,7 +6694,9 @@
       <c r="R97" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="S97" s="55"/>
+      <c r="S97" s="71" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="98" spans="1:19" s="64" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="55">
@@ -8074,7 +8078,7 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A2:O52"/>
+  <dimension ref="B2:O52"/>
   <sheetViews>
     <sheetView topLeftCell="A76" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>

</xml_diff>